<commit_message>
Funcionando pero PWM deficiente.
Former-commit-id: b166704ddf971e872be79b71a56732888cb00473
</commit_message>
<xml_diff>
--- a/Experiencia_5/seno.xlsx
+++ b/Experiencia_5/seno.xlsx
@@ -76,7 +76,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,53 +141,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="33" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="34">
+    <cellStyle name="Comma [0]" xfId="33" builtinId="6"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -539,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M57" sqref="I29:M57"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -550,11 +563,15 @@
     <col min="1" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="13" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -569,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16">
+    <row r="2" spans="1:10" ht="16">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -586,15 +603,15 @@
         <f>FLOOR(D2,1)</f>
         <v>16</v>
       </c>
-      <c r="F2" s="2">
-        <f>(D2-E2)*$H$7</f>
+      <c r="F2" s="5">
+        <f t="shared" ref="F2:F25" si="0">(D2-E2)*$H$7</f>
         <v>74403617.999999836</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" customHeight="1">
+    <row r="3" spans="1:10" ht="17" customHeight="1">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -608,11 +625,11 @@
         <v>17.73968838</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E25" si="0">FLOOR(D3,1)</f>
+        <f t="shared" ref="E3:E25" si="1">FLOOR(D3,1)</f>
         <v>17</v>
       </c>
-      <c r="F3" s="2">
-        <f>(D3-E3)*$H$7</f>
+      <c r="F3" s="5">
+        <f t="shared" si="0"/>
         <v>73968838.000000045</v>
       </c>
       <c r="H3" s="2">
@@ -620,7 +637,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17" customHeight="1">
+    <row r="4" spans="1:10" ht="17" customHeight="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -634,11 +651,11 @@
         <v>18.794545150000001</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F4" s="2">
-        <f>(D4-E4)*$H$7</f>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
         <v>79454515.000000119</v>
       </c>
       <c r="H4" s="2">
@@ -646,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17" customHeight="1">
+    <row r="5" spans="1:10" ht="17" customHeight="1">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -660,15 +677,15 @@
         <v>19.912126959999998</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="F5" s="2">
-        <f>(D5-E5)*$H$7</f>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
         <v>91212695.999999836</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" customHeight="1">
+    <row r="6" spans="1:10" ht="17" customHeight="1">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -682,18 +699,18 @@
         <v>21.09616364</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="F6" s="2">
-        <f>(D6-E6)*$H$7</f>
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
         <v>9616364.0000000335</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" customHeight="1">
+    <row r="7" spans="1:10" ht="17" customHeight="1">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -707,18 +724,26 @@
         <v>22.350606809999999</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="F7" s="2">
-        <f>(D7-E7)*$H$7</f>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
         <v>35060680.999999858</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
         <v>100000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" customHeight="1">
+      <c r="I7" s="5">
+        <f>2^28</f>
+        <v>268435456</v>
+      </c>
+      <c r="J7" s="5">
+        <f>I7-H7</f>
+        <v>168435456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" customHeight="1">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -732,11 +757,11 @@
         <v>23.679643049999999</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="F8" s="2">
-        <f>(D8-E8)*$H$7</f>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
         <v>67964304.999999925</v>
       </c>
       <c r="H8" s="2">
@@ -744,7 +769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" customHeight="1">
+    <row r="9" spans="1:10" ht="17" customHeight="1">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -758,15 +783,15 @@
         <v>25.087707900000002</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="F9" s="2">
-        <f>(D9-E9)*$H$7</f>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
         <v>8770790.0000001621</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" customHeight="1">
+    <row r="10" spans="1:10" ht="17" customHeight="1">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -780,15 +805,15 @@
         <v>26.57950065</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="F10" s="2">
-        <f>(D10-E10)*$H$7</f>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
         <v>57950064.999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
+    <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -802,15 +827,15 @@
         <v>28.16</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="F11" s="2">
-        <f>(D11-E11)*$H$7</f>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
         <v>16000000.000000015</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="17" customHeight="1">
+    <row r="12" spans="1:10" ht="17" customHeight="1">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -824,15 +849,15 @@
         <v>29.83448074</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="F12" s="2">
-        <f>(D12-E12)*$H$7</f>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
         <v>83448074</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" customHeight="1">
+    <row r="13" spans="1:10" ht="17" customHeight="1">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -846,15 +871,23 @@
         <v>31.608531280000001</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="F13" s="2">
-        <f>(D13-E13)*$H$7</f>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
         <v>60853128.000000112</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" customHeight="1">
+      <c r="H13" s="2">
+        <f>H7/H7</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <f>I7/H7</f>
+        <v>2.6843545600000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" customHeight="1">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -868,15 +901,15 @@
         <v>33.488072359999997</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="F14" s="2">
-        <f>(D14-E14)*$H$7</f>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
         <v>48807235.99999968</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17" customHeight="1">
+    <row r="15" spans="1:10" ht="17" customHeight="1">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -890,15 +923,15 @@
         <v>35.479376770000002</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="F15" s="2">
-        <f>(D15-E15)*$H$7</f>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
         <v>47937677.000000179</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17" customHeight="1">
+    <row r="16" spans="1:10" ht="17" customHeight="1">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -912,15 +945,15 @@
         <v>37.589090290000001</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="F16" s="2">
-        <f>(D16-E16)*$H$7</f>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
         <v>58909029.000000149</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1">
+    <row r="17" spans="1:9" ht="17" customHeight="1">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -934,15 +967,15 @@
         <v>39.824253919999997</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="F17" s="2">
-        <f>(D17-E17)*$H$7</f>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
         <v>82425391.999999672</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1">
+    <row r="18" spans="1:9" ht="17" customHeight="1">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -956,15 +989,15 @@
         <v>42.192327280000001</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="F18" s="2">
-        <f>(D18-E18)*$H$7</f>
+      <c r="F18" s="5">
+        <f t="shared" si="0"/>
         <v>19232728.000000067</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1">
+    <row r="19" spans="1:9" ht="17" customHeight="1">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -978,15 +1011,15 @@
         <v>44.701213619999997</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="F19" s="2">
-        <f>(D19-E19)*$H$7</f>
+      <c r="F19" s="5">
+        <f t="shared" si="0"/>
         <v>70121361.999999717</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1">
+    <row r="20" spans="1:9" ht="17" customHeight="1">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1000,15 +1033,15 @@
         <v>47.359286109999999</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="F20" s="2">
-        <f>(D20-E20)*$H$7</f>
+      <c r="F20" s="5">
+        <f t="shared" si="0"/>
         <v>35928610.999999933</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1">
+    <row r="21" spans="1:9" ht="17" customHeight="1">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1022,15 +1055,15 @@
         <v>50.175415809999997</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F21" s="2">
-        <f>(D21-E21)*$H$7</f>
+      <c r="F21" s="5">
+        <f t="shared" si="0"/>
         <v>17541580.999999695</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1">
+    <row r="22" spans="1:9" ht="17" customHeight="1">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1044,15 +1077,15 @@
         <v>53.159001289999999</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="F22" s="2">
-        <f>(D22-E22)*$H$7</f>
+      <c r="F22" s="5">
+        <f t="shared" si="0"/>
         <v>15900128.999999907</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1066,15 +1099,15 @@
         <v>56.32</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="F23" s="2">
-        <f>(D23-E23)*$H$7</f>
+      <c r="F23" s="5">
+        <f t="shared" si="0"/>
         <v>32000000.00000003</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17" customHeight="1">
+    <row r="24" spans="1:9" ht="17" customHeight="1">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1088,15 +1121,15 @@
         <v>59.668961469999999</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="F24" s="2">
-        <f>(D24-E24)*$H$7</f>
+      <c r="F24" s="5">
+        <f t="shared" si="0"/>
         <v>66896146.999999925</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1">
+    <row r="25" spans="1:9" ht="17" customHeight="1">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1110,16 +1143,28 @@
         <v>63.217062560000002</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="F25" s="2">
-        <f>(D25-E25)*$H$7</f>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
         <v>21706256.000000224</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:9">
       <c r="F26" s="4"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="I30" s="5">
+        <f>2^29</f>
+        <v>536870912</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9">
+      <c r="I36" s="2">
+        <f>2^9</f>
+        <v>512</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>